<commit_message>
Corrigido valor de R49 e outros pequenos detalhes
</commit_message>
<xml_diff>
--- a/Rev6/Docs/BOM.xlsx
+++ b/Rev6/Docs/BOM.xlsx
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>28</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Adicionado fotos da placa Rev 7 montada Alterado instruções para formato Markdown Corrigido capacitor C1 na placa rev. 7 Outras pequenas melhorias e correções
</commit_message>
<xml_diff>
--- a/Rev6/Docs/BOM.xlsx
+++ b/Rev6/Docs/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>Resistores (1/4W)</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>47K</t>
+  </si>
+  <si>
+    <t>OBSERVAÇÕES</t>
+  </si>
+  <si>
+    <t>Se for montar com 32K de RAM alta, reduzir um</t>
+  </si>
+  <si>
+    <t>diodos 1N4148 (comprar somente 22)</t>
+  </si>
+  <si>
+    <t>resistor de 1K (comprar somente 4) e reduzir dois</t>
   </si>
 </sst>
 </file>
@@ -274,12 +286,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -294,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -313,6 +331,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,10 +939,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="7">
         <v>24</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1071,45 +1095,61 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
       <c r="B36" s="4">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E36" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>5</v>
       </c>
       <c r="B37" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
       <c r="B38" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -1117,7 +1157,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>24</v>
       </c>
@@ -1125,7 +1165,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -1133,15 +1173,15 @@
         <v>680</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>5</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2</v>
       </c>
@@ -1149,7 +1189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -1157,7 +1197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>12</v>
       </c>
@@ -1165,7 +1205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>13</v>
       </c>
@@ -1173,7 +1213,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -1181,7 +1221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Adicionado soquetes na lista de material versão em excel. Refeito gerbers e mapa da revisão 7
</commit_message>
<xml_diff>
--- a/Rev6/Docs/BOM.xlsx
+++ b/Rev6/Docs/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>Resistores (1/4W)</t>
   </si>
@@ -255,6 +255,27 @@
   </si>
   <si>
     <t>resistor de 1K (comprar somente 4) e reduzir dois</t>
+  </si>
+  <si>
+    <t>Soquetes</t>
+  </si>
+  <si>
+    <t>40 pinos</t>
+  </si>
+  <si>
+    <t>28 pinos largo</t>
+  </si>
+  <si>
+    <t>20 pinos</t>
+  </si>
+  <si>
+    <t>18 pinos</t>
+  </si>
+  <si>
+    <t>16 pinos</t>
+  </si>
+  <si>
+    <t>14 pinos</t>
   </si>
 </sst>
 </file>
@@ -312,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -326,6 +347,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -335,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +648,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,25 +663,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -900,17 +927,17 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="8"/>
       <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
@@ -939,10 +966,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="5">
         <v>24</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -961,11 +988,11 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
@@ -979,10 +1006,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="8"/>
       <c r="D26" s="1">
         <v>1</v>
       </c>
@@ -1096,10 +1123,15 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1108,10 +1140,13 @@
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="7"/>
+      <c r="D35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1120,10 +1155,12 @@
       <c r="B36" s="4">
         <v>75</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -1132,10 +1169,12 @@
       <c r="B37" s="4">
         <v>100</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="7"/>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -1144,10 +1183,12 @@
       <c r="B38" s="4">
         <v>150</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="7"/>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -1155,6 +1196,12 @@
       </c>
       <c r="B39" s="4">
         <v>220</v>
+      </c>
+      <c r="D39" s="1">
+        <v>5</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1164,6 +1211,12 @@
       <c r="B40" s="4">
         <v>470</v>
       </c>
+      <c r="D40" s="1">
+        <v>12</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -1172,12 +1225,18 @@
       <c r="B41" s="4">
         <v>680</v>
       </c>
+      <c r="D41" s="1">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+      <c r="A42" s="5">
         <v>5</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1204,6 +1263,11 @@
       <c r="B45" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="D45" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -1212,6 +1276,11 @@
       <c r="B46" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="D46" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -1220,6 +1289,11 @@
       <c r="B47" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="D47" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -1228,9 +1302,19 @@
       <c r="B48" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="D48" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D34:F34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="A34:B34"/>

</xml_diff>